<commit_message>
Deploying to gh-pages from  @ 693af5ca6946a40afa29b0598b9815a47090caa4 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.1.1.1e.xlsx
+++ b/en/downloads/data-excel/2.1.1.1e.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Национальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Национальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -554,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,7 +564,7 @@
     <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -584,7 +584,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -604,7 +604,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -618,8 +618,9 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -659,8 +660,11 @@
       <c r="M4" s="5">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="N4" s="5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -698,10 +702,13 @@
         <v>65.742251223491024</v>
       </c>
       <c r="M5" s="10">
-        <v>69.168026101141919</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="N5" s="10">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -739,10 +746,13 @@
         <v>109.4</v>
       </c>
       <c r="M6" s="10">
-        <v>109.85000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>108.2</v>
+      </c>
+      <c r="N6" s="10">
+        <v>106.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -780,10 +790,13 @@
         <v>47.342465753424662</v>
       </c>
       <c r="M7" s="10">
-        <v>52.219178082191775</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>51.7</v>
+      </c>
+      <c r="N7" s="10">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -821,10 +834,13 @@
         <v>115.234375</v>
       </c>
       <c r="M8" s="10">
-        <v>98.437499999999986</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>97.7</v>
+      </c>
+      <c r="N8" s="10">
+        <v>49.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -859,13 +875,16 @@
         <v>112.81489594742607</v>
       </c>
       <c r="L9" s="10">
-        <v>104.052573932092</v>
+        <v>105.6</v>
       </c>
       <c r="M9" s="10">
-        <v>106.24315443592552</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>106.7</v>
+      </c>
+      <c r="N9" s="10">
+        <v>108.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -903,10 +922,13 @@
         <v>141.98782961460446</v>
       </c>
       <c r="M10" s="10">
-        <v>125.55780933062881</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>124.2</v>
+      </c>
+      <c r="N10" s="10">
+        <v>107.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -944,10 +966,13 @@
         <v>158.88013998250219</v>
       </c>
       <c r="M11" s="10">
-        <v>140.24496937882768</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="N11" s="10">
+        <v>155.69999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
@@ -982,13 +1007,16 @@
         <v>34.5</v>
       </c>
       <c r="L12" s="10">
-        <v>27</v>
+        <v>27.1</v>
       </c>
       <c r="M12" s="10">
-        <v>34.195634599838314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33.9</v>
+      </c>
+      <c r="N12" s="10">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -1026,10 +1054,13 @@
         <v>99.071585634009267</v>
       </c>
       <c r="M13" s="10">
-        <v>96.994869289030063</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="N13" s="10">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
@@ -1067,10 +1098,14 @@
         <v>8.791208791208792</v>
       </c>
       <c r="M14" s="12">
-        <v>6.593406593406594</v>
+        <v>7.7</v>
+      </c>
+      <c r="N14" s="12">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>